<commit_message>
Primeiro commit no novo reposritorio
</commit_message>
<xml_diff>
--- a/POC CONSTRUMAQ/POC CONSTRUMAQ/TEST/static/dados_de_pagamento.xlsx
+++ b/POC CONSTRUMAQ/POC CONSTRUMAQ/TEST/static/dados_de_pagamento.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Dados do Funcionário" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados do Funcionário" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,20 +429,30 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Funcao</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>equipe</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Chave PIX</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Valor Total</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Data de Pagamento</t>
         </is>
@@ -451,298 +461,173 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ALEXANDRE MACHADO DE MORAES</t>
+          <t>TESTE DE BUG 9</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01455194220</t>
+          <t>TESTE 1230909</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>f19b19aa-e417-4c82-b0c7-ea2a784b0a48</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>628.38</v>
+          <t>Dentista</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>89899898989</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>08/11/2024</t>
+          <t>87888</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>6980.13</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>12/11/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BRUNO ACACIO VIEIRA</t>
+          <t>FELIPE VENCEDOR 7</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>71253121281</t>
+          <t>DESENVOLVEDOR PLENO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TEL: (91)98244-0145</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2483.17390656</v>
+          <t>Equipe 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>09090909090</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>8090909</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>594</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>06/11/2024</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DANIEL NUNES GUEDES</t>
+          <t>BRUNO ACACIO VIEIRA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>91941415253</t>
+          <t>Eletricista</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CPF: 91941415253</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>2485.31928144</v>
+          <t>Eletricista</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>71253121281</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>TEL: (91)98244-0145</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>637.85</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>15/11/2024</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FATIMA PEREIRA</t>
+          <t>FREDSON MAUES SERRÃO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>88593770215</t>
+          <t>SERVENTE HABILITADO</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CNPJ: 56144061000187</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>-498520.3339113744</v>
+          <t>EQUIPE LENILSON</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>02178798292</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>TEL: (94)98813-0744</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>155.14</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>15/11/2024</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>LUIZ GERALDO DA CONCEICAO DE ALEXANDRIA</t>
+          <t>MATEUS GUSMA DE SA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>39558387204</t>
+          <t>SERVENTE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Tel: (91) 98166-6402</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>638.4</v>
+          <t>EQUIPE GALPÃO</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>04369577284</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>06/12/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>081f2d7b-93d9-41b3-85bc-0511a97b8f71</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>89899898989</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>87888</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>4676.68</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>21/11/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ALEXANDRE MACHADO DE teste</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>98909090909</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>00</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>08/11/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>373781dd-491d-4263-93dc-0fb001ce919a</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>09090909090</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>9890980989</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>1646.23</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>08/11/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>4c72ff85-bd80-4b1c-8e1a-57ee7f35ba97</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>09090909090</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>9090909</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>6481.72</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>21/11/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>428bfef8-09de-46d7-92db-19bc76a01d05</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>01455194220</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>f19b19aa-e417-4c82-b0c7-ea2a784b0a48</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>628.38</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>21/11/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>a8381105-5054-4954-8076-9b95da57538f</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>90909098898</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>TESTE@TESTE.COM</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>611.37</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>15/11/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>FELIP RENAN RODRIGUES DOS SANTOS</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>90909098898</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>TESTE@TESTE.COM</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>635.1900000000001</v>
-      </c>
-      <c r="E13" t="inlineStr">
+          <t>TEL:(91)98477-1882</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>416.64</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>15/11/2024</t>
         </is>

</xml_diff>